<commit_message>
added testplan to set control register mode
</commit_message>
<xml_diff>
--- a/testplan_spi.xlsx
+++ b/testplan_spi.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="8355"/>
+    <workbookView windowWidth="15990" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
   <si>
-    <t>SPI VIP VERIFICATION PLAN</t>
+    <r>
+      <t xml:space="preserve">                             </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SPI VIP VERIFICATION PLAN</t>
+    </r>
   </si>
   <si>
     <t>SL_NO</t>
@@ -28,20 +41,105 @@
     <t xml:space="preserve">   VERIFICATION CRITERIA</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>SETTING SPIE AND MSTR BITS IN CONTROL REGISTER</t>
   </si>
   <si>
-    <t>setting the 6th and 4th bit of control registers.           If SPE is 1 system is on.                                                           If MSTR is 0, slave mode (MOSI).                                                         If MSTR is 1, master mode(MISO).</t>
+    <r>
+      <t xml:space="preserve">Setting the 6th and 4th bit of control registers. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">       
+If SPE is 1 system is on.                                                                                 If MSTR is 0, slave mode (MOSI).                                                             If MSTR is 1, master mode(MISO).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+SET THE MODE OF SPI CONTROL REGISTER
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                    
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Setting the 3rd and 2nd bit of spi control register
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+CPOL bit,clock polarity and CPHASE bit clockphase .
+MODE 0:If CPOL==0&amp;&amp;CPHASE==0,the data is sampled at posedge of clock and active state of clk is 1,
+MODE 1:If CPOL==0&amp;&amp;CPHASE==1,data is sampled at trailing edge of the clock and active state of clk is 0,
+MODE2:If CPOL==1&amp;&amp;CPHASE==1,data is sampled at posedge of clk,active state of clk is 0,                              
+MODE 3:If CPOL==1&amp;&amp;CPHASE==1,data is sampled at trailing edge of clk and active state of the clk is 0   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,22 +149,379 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -93,9 +548,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -109,29 +562,429 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -393,62 +1246,76 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.4190476190476" customWidth="1"/>
+    <col min="3" max="3" width="57.8095238095238" customWidth="1"/>
+    <col min="4" max="4" width="62.647619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="22.5">
-      <c r="B2" s="1" t="s">
+    <row r="3" ht="25.5" spans="3:3">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="3:4">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" ht="38" customHeight="1" spans="2:4">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="6" customFormat="1" ht="60">
-      <c r="A7" s="5">
+    <row r="7" s="1" customFormat="1" ht="202" customHeight="1" spans="1:4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+    </row>
+    <row r="8" s="2" customFormat="1" ht="233" customHeight="1" spans="2:4">
+      <c r="B8" s="12">
+        <v>2</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>4</v>
+      <c r="D8" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
+    <row r="9" ht="208" customHeight="1" spans="2:4">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>